<commit_message>
fix: missing dep for excel reading
</commit_message>
<xml_diff>
--- a/input/data.local/lit_dengue_out_loc/WHOAB_summary_withSignalSheet.xlsx
+++ b/input/data.local/lit_dengue_out_loc/WHOAB_summary_withSignalSheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jona/htdocs/MARS/esida-db/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jona/htdocs/MARS/esida-db/input/data.local/lit_dengue_out_loc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C1F49B-0430-B944-85A5-B01474E70E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28ED5832-5C56-2347-89A9-58F31A2D9934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30240" yWindow="-3860" windowWidth="38400" windowHeight="23500" activeTab="1" xr2:uid="{4FDD09CF-70D4-0745-8605-751E8E3374B3}"/>
   </bookViews>
@@ -560,9 +560,6 @@
     <t>WHOWB.18.A.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Report date </t>
-  </si>
-  <si>
     <t>Start date</t>
   </si>
   <si>
@@ -623,9 +620,6 @@
     <t>WHOWB.19.A.13</t>
   </si>
   <si>
-    <t>Ruvama</t>
-  </si>
-  <si>
     <t>Lindi</t>
   </si>
   <si>
@@ -665,9 +659,6 @@
     <t>WHOWB.19.A.23</t>
   </si>
   <si>
-    <t>Dodorma</t>
-  </si>
-  <si>
     <t>Kagera</t>
   </si>
   <si>
@@ -677,13 +668,22 @@
     <t>Ruvuma</t>
   </si>
   <si>
-    <t>Sinigda</t>
-  </si>
-  <si>
     <t>WHOWB.19.A.24</t>
   </si>
   <si>
     <t>Regions</t>
+  </si>
+  <si>
+    <t>Singida</t>
+  </si>
+  <si>
+    <t>Dar-es-salaam</t>
+  </si>
+  <si>
+    <t>Dodoma</t>
+  </si>
+  <si>
+    <t>Report date</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1168,7 @@
   <dimension ref="A1:K265"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H143" sqref="H143"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9977,7 +9977,7 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9994,10 +9994,10 @@
         <v>148</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>193</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>152</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>6</v>
@@ -10009,10 +10009,10 @@
         <v>8</v>
       </c>
       <c r="G1" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="17" t="s">
         <v>153</v>
-      </c>
-      <c r="H1" s="17" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -10020,7 +10020,7 @@
         <v>150</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C2" s="10">
         <v>41782</v>
@@ -10124,7 +10124,7 @@
         <v>151</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C6" s="10">
         <v>43182</v>
@@ -10147,10 +10147,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C7" s="10">
         <v>43280</v>
@@ -10173,10 +10173,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C8" s="10">
         <v>43287</v>
@@ -10199,10 +10199,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C9" s="16">
         <v>43497</v>
@@ -10225,10 +10225,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="C10" s="16">
         <v>43497</v>
@@ -10251,10 +10251,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C11" s="16">
         <v>43506</v>
@@ -10277,10 +10277,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="C12" s="16">
         <v>43506</v>
@@ -10305,10 +10305,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C13" s="16">
         <v>43534</v>
@@ -10331,10 +10331,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C14" s="16">
         <v>43534</v>
@@ -10357,10 +10357,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C15" s="16">
         <v>43569</v>
@@ -10383,10 +10383,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C16" s="16">
         <v>43569</v>
@@ -10409,10 +10409,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C17" s="16">
         <v>43576</v>
@@ -10435,10 +10435,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C18" s="16">
         <v>43576</v>
@@ -10464,10 +10464,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C19" s="16">
         <v>43583</v>
@@ -10490,10 +10490,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C20" s="16">
         <v>43583</v>
@@ -10516,10 +10516,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C21" s="10">
         <v>43597</v>
@@ -10542,10 +10542,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C22" s="10">
         <v>43597</v>
@@ -10571,10 +10571,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C23" s="10">
         <v>43604</v>
@@ -10597,10 +10597,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C24" s="10">
         <v>43611</v>
@@ -10623,10 +10623,10 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C25" s="10">
         <v>43618</v>
@@ -10649,10 +10649,10 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C26" s="10">
         <v>43618</v>
@@ -10678,10 +10678,10 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>166</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>167</v>
       </c>
       <c r="C27" s="10">
         <v>43618</v>
@@ -10707,10 +10707,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C28" s="10">
         <v>43618</v>
@@ -10736,10 +10736,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C29" s="10">
         <v>43632</v>
@@ -10762,10 +10762,10 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C30" s="10">
         <v>43632</v>
@@ -10788,10 +10788,10 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C31" s="10">
         <v>43632</v>
@@ -10814,10 +10814,10 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" s="10">
         <v>43632</v>
@@ -10840,10 +10840,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C33" s="10">
         <v>43639</v>
@@ -10866,10 +10866,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C34" s="10">
         <v>43639</v>
@@ -10895,10 +10895,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C35" s="10">
         <v>43639</v>
@@ -10924,10 +10924,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C36" s="10">
         <v>43639</v>
@@ -10953,10 +10953,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C37" s="10">
         <v>43646</v>
@@ -10979,10 +10979,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C38" s="10">
         <v>43646</v>
@@ -11005,10 +11005,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C39" s="10">
         <v>43646</v>
@@ -11031,10 +11031,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="10">
         <v>43646</v>
@@ -11057,10 +11057,10 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C41" s="10">
         <v>43653</v>
@@ -11083,10 +11083,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C42" s="10">
         <v>43653</v>
@@ -11109,10 +11109,10 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C43" s="10">
         <v>43653</v>
@@ -11135,10 +11135,10 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C44" s="10">
         <v>43653</v>
@@ -11161,10 +11161,10 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="C45" s="10">
         <v>43653</v>
@@ -11187,10 +11187,10 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C46" s="10">
         <v>43660</v>
@@ -11213,10 +11213,10 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C47" s="10">
         <v>43660</v>
@@ -11239,10 +11239,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C48" s="10">
         <v>43660</v>
@@ -11265,10 +11265,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C49" s="10">
         <v>43660</v>
@@ -11291,10 +11291,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="C50" s="10">
         <v>43660</v>
@@ -11317,10 +11317,10 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C51" s="10">
         <v>43667</v>
@@ -11343,10 +11343,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C52" s="10">
         <v>43667</v>
@@ -11369,10 +11369,10 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C53" s="10">
         <v>43667</v>
@@ -11395,10 +11395,10 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C54" s="10">
         <v>43667</v>
@@ -11421,10 +11421,10 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C55" s="10">
         <v>43674</v>
@@ -11447,10 +11447,10 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C56" s="10">
         <v>43675</v>
@@ -11473,10 +11473,10 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C57" s="10">
         <v>43676</v>
@@ -11499,10 +11499,10 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C58" s="10">
         <v>43677</v>
@@ -11525,10 +11525,10 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C59" s="10">
         <v>43688</v>
@@ -11551,10 +11551,10 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C60" s="10">
         <v>43688</v>
@@ -11577,10 +11577,10 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B61" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C61" s="10">
         <v>43695</v>
@@ -11603,10 +11603,10 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C62" s="10">
         <v>43695</v>
@@ -11624,15 +11624,15 @@
         <v>43313</v>
       </c>
       <c r="H62" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C63" s="10">
         <v>43702</v>
@@ -11655,10 +11655,10 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C64" s="10">
         <v>43702</v>
@@ -11681,10 +11681,10 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C65" s="10">
         <v>43709</v>
@@ -11707,10 +11707,10 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C66" s="10">
         <v>43709</v>
@@ -11733,10 +11733,10 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C67" s="10">
         <v>43716</v>
@@ -11759,10 +11759,10 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C68" s="10">
         <v>43716</v>
@@ -11785,10 +11785,10 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C69" s="10">
         <v>43723</v>
@@ -11811,10 +11811,10 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C70" s="10">
         <v>43723</v>
@@ -11837,10 +11837,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C71" s="10">
         <v>43744</v>
@@ -11863,10 +11863,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C72" s="10">
         <v>43744</v>
@@ -11889,10 +11889,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="C73" s="10">
         <v>43744</v>
@@ -11915,10 +11915,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B74" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C74" s="10">
         <v>43744</v>
@@ -11941,10 +11941,10 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="B75" s="10" t="s">
         <v>186</v>
-      </c>
-      <c r="B75" s="10" t="s">
-        <v>189</v>
       </c>
       <c r="C75" s="10">
         <v>43744</v>
@@ -11967,10 +11967,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C76" s="10">
         <v>43744</v>
@@ -11993,10 +11993,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C77" s="10">
         <v>43744</v>
@@ -12019,10 +12019,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C78" s="10">
         <v>43744</v>
@@ -12045,10 +12045,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C79" s="10">
         <v>43744</v>
@@ -12071,10 +12071,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C80" s="10">
         <v>43744</v>
@@ -12097,10 +12097,10 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C81" s="10">
         <v>43758</v>
@@ -12123,10 +12123,10 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>92</v>
+        <v>191</v>
       </c>
       <c r="C82" s="10">
         <v>43758</v>
@@ -12149,10 +12149,10 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="B83" s="10" t="s">
         <v>192</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>187</v>
       </c>
       <c r="C83" s="10">
         <v>43758</v>
@@ -12175,10 +12175,10 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C84" s="10">
         <v>43758</v>
@@ -12201,10 +12201,10 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C85" s="10">
         <v>43758</v>
@@ -12227,10 +12227,10 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C86" s="10">
         <v>43758</v>
@@ -12253,10 +12253,10 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C87" s="10">
         <v>43758</v>
@@ -12280,10 +12280,10 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B88" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C88" s="10">
         <v>43758</v>
@@ -12307,10 +12307,10 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B89" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C89" s="10">
         <v>43758</v>
@@ -12334,10 +12334,10 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C90" s="10">
         <v>43758</v>

</xml_diff>